<commit_message>
Fix: update db model
</commit_message>
<xml_diff>
--- a/app/data/static/params/mascarpone.xlsx
+++ b/app/data/static/params/mascarpone.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="151">
   <si>
     <t xml:space="preserve">Название SKU</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t xml:space="preserve">Вес</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Вес технология</t>
   </si>
   <si>
     <t xml:space="preserve">Коробки</t>
@@ -479,7 +482,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -508,18 +511,6 @@
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <name val="Cambria"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -577,7 +568,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -586,15 +577,11 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -611,23 +598,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF3D3D3D"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
 </styleSheet>
 </file>
 
@@ -636,13 +606,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V53"/>
+  <dimension ref="A1:W53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R1" activeCellId="0" sqref="R1"/>
+      <selection pane="topLeft" activeCell="H22" activeCellId="0" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.69"/>
   </cols>
@@ -690,7 +660,7 @@
       <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="Q1" s="1" t="s">
@@ -711,68 +681,74 @@
       <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="W1" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>80</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I2" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="J2" s="0" t="n">
-        <v>6</v>
+        <v>0.2</v>
       </c>
       <c r="K2" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L2" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="N2" s="0" t="n">
-        <v>50</v>
-      </c>
       <c r="O2" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="P2" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="P2" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="Q2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="R2" s="0" t="n">
-        <v>600</v>
-      </c>
-      <c r="S2" s="3"/>
-      <c r="T2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="T2" s="2"/>
+      <c r="U2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V2" s="0" t="s">
-        <v>25</v>
+      <c r="V2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -780,62 +756,65 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>80</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I3" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="J3" s="0" t="n">
-        <v>6</v>
+        <v>0.2</v>
       </c>
       <c r="K3" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L3" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="N3" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="O3" s="4" t="n">
+      <c r="O3" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="P3" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="P3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R3" s="0" t="n">
-        <v>600</v>
-      </c>
-      <c r="S3" s="3"/>
-      <c r="T3" s="0" t="n">
+      <c r="Q3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="T3" s="2"/>
+      <c r="U3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V3" s="0" t="s">
-        <v>28</v>
+      <c r="V3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -843,62 +822,65 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>80</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I4" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="J4" s="0" t="n">
-        <v>6</v>
+        <v>0.5</v>
       </c>
       <c r="K4" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L4" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="N4" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="O4" s="4" t="n">
+      <c r="O4" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="P4" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="P4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R4" s="0" t="n">
+      <c r="Q4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" s="0" t="n">
         <v>1400</v>
       </c>
-      <c r="S4" s="3"/>
-      <c r="T4" s="0" t="n">
+      <c r="T4" s="2"/>
+      <c r="U4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V4" s="0" t="s">
-        <v>30</v>
+      <c r="V4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W4" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -906,62 +888,65 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>80</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="J5" s="0" t="n">
-        <v>6</v>
+        <v>0.2</v>
       </c>
       <c r="K5" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L5" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="N5" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="O5" s="4" t="n">
+      <c r="O5" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="P5" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="P5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R5" s="0" t="n">
-        <v>600</v>
-      </c>
-      <c r="S5" s="3"/>
-      <c r="T5" s="0" t="n">
+      <c r="Q5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="T5" s="2"/>
+      <c r="U5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V5" s="0" t="s">
-        <v>33</v>
+      <c r="V5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W5" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -969,65 +954,68 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>50</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>0.2</v>
       </c>
       <c r="J6" s="0" t="n">
-        <v>6</v>
+        <v>0.2</v>
       </c>
       <c r="K6" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L6" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="N6" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="O6" s="4" t="n">
+      <c r="O6" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="P6" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="P6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="4" t="n">
+      <c r="Q6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="R6" s="0" t="n">
-        <v>600</v>
-      </c>
-      <c r="S6" s="3"/>
-      <c r="T6" s="0" t="n">
+      <c r="S6" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="T6" s="2"/>
+      <c r="U6" s="0" t="n">
         <v>1.5</v>
       </c>
-      <c r="U6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V6" s="0" t="s">
-        <v>36</v>
+      <c r="V6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W6" s="0" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1035,62 +1023,65 @@
         <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>80</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="J7" s="0" t="n">
-        <v>6</v>
+        <v>0.2</v>
       </c>
       <c r="K7" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L7" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="N7" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="O7" s="4" t="n">
+      <c r="O7" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="P7" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="P7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R7" s="0" t="n">
-        <v>600</v>
-      </c>
-      <c r="S7" s="3"/>
-      <c r="T7" s="0" t="n">
+      <c r="Q7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="T7" s="2"/>
+      <c r="U7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V7" s="0" t="s">
-        <v>39</v>
+      <c r="V7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W7" s="0" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1098,62 +1089,65 @@
         <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>80</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="J8" s="0" t="n">
-        <v>6</v>
+        <v>0.2</v>
       </c>
       <c r="K8" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L8" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="N8" s="0" t="n">
-        <v>50</v>
-      </c>
       <c r="O8" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="P8" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="P8" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="Q8" s="0" t="n">
         <v>0</v>
       </c>
       <c r="R8" s="0" t="n">
-        <v>600</v>
-      </c>
-      <c r="S8" s="3"/>
-      <c r="T8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="T8" s="2"/>
+      <c r="U8" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V8" s="0" t="s">
-        <v>42</v>
+      <c r="V8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W8" s="0" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1161,62 +1155,65 @@
         <v>7</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>80</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="J9" s="0" t="n">
-        <v>6</v>
+        <v>0.5</v>
       </c>
       <c r="K9" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L9" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="N9" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="O9" s="4" t="n">
+      <c r="O9" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="P9" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="P9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R9" s="0" t="n">
+      <c r="Q9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" s="0" t="n">
         <v>1400</v>
       </c>
-      <c r="S9" s="3"/>
-      <c r="T9" s="0" t="n">
+      <c r="T9" s="2"/>
+      <c r="U9" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V9" s="0" t="s">
-        <v>45</v>
+      <c r="V9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W9" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1224,65 +1221,68 @@
         <v>8</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>50</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>0.2</v>
       </c>
       <c r="J10" s="0" t="n">
-        <v>6</v>
+        <v>0.2</v>
       </c>
       <c r="K10" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L10" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="N10" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="O10" s="4" t="n">
+      <c r="O10" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="P10" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="P10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="4" t="n">
+      <c r="Q10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R10" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="R10" s="0" t="n">
-        <v>600</v>
-      </c>
-      <c r="S10" s="3"/>
-      <c r="T10" s="0" t="n">
+      <c r="S10" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="T10" s="2"/>
+      <c r="U10" s="0" t="n">
         <v>1.5</v>
       </c>
-      <c r="U10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V10" s="0" t="s">
-        <v>48</v>
+      <c r="V10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W10" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1290,62 +1290,65 @@
         <v>9</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>38</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I11" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="J11" s="0" t="n">
-        <v>6</v>
+        <v>0.5</v>
       </c>
       <c r="K11" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="M11" s="0" t="n">
-        <v>20</v>
-      </c>
       <c r="N11" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="O11" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R11" s="5" t="n">
+      <c r="O11" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="P11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" s="4" t="n">
         <v>1400</v>
       </c>
-      <c r="S11" s="3"/>
-      <c r="T11" s="0" t="n">
+      <c r="T11" s="2"/>
+      <c r="U11" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U11" s="0" t="n">
+      <c r="V11" s="0" t="n">
         <v>-100</v>
       </c>
-      <c r="V11" s="0" t="s">
-        <v>51</v>
+      <c r="W11" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1353,62 +1356,65 @@
         <v>10</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>38</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I12" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="J12" s="0" t="n">
-        <v>6</v>
+        <v>0.2</v>
       </c>
       <c r="K12" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="M12" s="0" t="n">
-        <v>20</v>
-      </c>
       <c r="N12" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="O12" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R12" s="0" t="n">
-        <v>600</v>
-      </c>
-      <c r="S12" s="3"/>
-      <c r="T12" s="0" t="n">
+      <c r="O12" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="P12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="T12" s="2"/>
+      <c r="U12" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U12" s="0" t="n">
+      <c r="V12" s="0" t="n">
         <v>-100</v>
       </c>
-      <c r="V12" s="0" t="s">
-        <v>53</v>
+      <c r="W12" s="0" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1416,62 +1422,65 @@
         <v>11</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>38</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I13" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="J13" s="0" t="n">
-        <v>6</v>
+        <v>0.2</v>
       </c>
       <c r="K13" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="M13" s="0" t="n">
-        <v>20</v>
-      </c>
       <c r="N13" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="O13" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R13" s="0" t="n">
-        <v>600</v>
-      </c>
-      <c r="S13" s="3"/>
-      <c r="T13" s="0" t="n">
+      <c r="O13" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="P13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="T13" s="2"/>
+      <c r="U13" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U13" s="0" t="n">
+      <c r="V13" s="0" t="n">
         <v>-100</v>
       </c>
-      <c r="V13" s="0" t="s">
-        <v>55</v>
+      <c r="W13" s="0" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1479,62 +1488,65 @@
         <v>12</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>80</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I14" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="J14" s="0" t="n">
-        <v>6</v>
+        <v>0.2</v>
       </c>
       <c r="K14" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L14" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="N14" s="0" t="n">
-        <v>50</v>
-      </c>
       <c r="O14" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="P14" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="P14" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="Q14" s="0" t="n">
         <v>0</v>
       </c>
       <c r="R14" s="0" t="n">
-        <v>600</v>
-      </c>
-      <c r="S14" s="3"/>
-      <c r="T14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S14" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="T14" s="2"/>
+      <c r="U14" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V14" s="0" t="s">
-        <v>58</v>
+      <c r="V14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W14" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1542,62 +1554,65 @@
         <v>13</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>80</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I15" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="J15" s="0" t="n">
-        <v>6</v>
+        <v>0.2</v>
       </c>
       <c r="K15" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L15" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="N15" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="O15" s="4" t="n">
+      <c r="O15" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="P15" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="P15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R15" s="0" t="n">
-        <v>600</v>
-      </c>
-      <c r="S15" s="3"/>
-      <c r="T15" s="0" t="n">
+      <c r="Q15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R15" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S15" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="T15" s="2"/>
+      <c r="U15" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V15" s="0" t="s">
-        <v>60</v>
+      <c r="V15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W15" s="0" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1605,65 +1620,68 @@
         <v>14</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>50</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I16" s="0" t="n">
         <v>0.14</v>
       </c>
       <c r="J16" s="0" t="n">
-        <v>6</v>
+        <v>0.2</v>
       </c>
       <c r="K16" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L16" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="N16" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="O16" s="4" t="n">
+      <c r="O16" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="P16" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="P16" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="4" t="n">
+      <c r="Q16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R16" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="R16" s="0" t="n">
-        <v>600</v>
-      </c>
-      <c r="S16" s="3"/>
-      <c r="T16" s="0" t="n">
+      <c r="S16" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="T16" s="2"/>
+      <c r="U16" s="0" t="n">
         <v>1.5</v>
       </c>
-      <c r="U16" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V16" s="0" t="s">
-        <v>62</v>
+      <c r="V16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W16" s="0" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1671,62 +1689,65 @@
         <v>15</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>38</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I17" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="J17" s="0" t="n">
-        <v>6</v>
+        <v>0.5</v>
       </c>
       <c r="K17" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="M17" s="0" t="n">
-        <v>20</v>
-      </c>
       <c r="N17" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="O17" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R17" s="0" t="n">
+      <c r="O17" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="P17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S17" s="0" t="n">
         <v>1400</v>
       </c>
-      <c r="S17" s="3"/>
-      <c r="T17" s="0" t="n">
+      <c r="T17" s="2"/>
+      <c r="U17" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U17" s="0" t="n">
+      <c r="V17" s="0" t="n">
         <v>-100</v>
       </c>
-      <c r="V17" s="0" t="s">
-        <v>64</v>
+      <c r="W17" s="0" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1734,62 +1755,65 @@
         <v>16</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>80</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I18" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="J18" s="0" t="n">
-        <v>6</v>
+        <v>0.2</v>
       </c>
       <c r="K18" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L18" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="N18" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="O18" s="4" t="n">
+      <c r="O18" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="P18" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="P18" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R18" s="0" t="n">
-        <v>600</v>
-      </c>
-      <c r="S18" s="3"/>
-      <c r="T18" s="0" t="n">
+      <c r="Q18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R18" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S18" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="T18" s="2"/>
+      <c r="U18" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U18" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V18" s="0" t="s">
-        <v>66</v>
+      <c r="V18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W18" s="0" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1797,62 +1821,65 @@
         <v>17</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>38</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I19" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="J19" s="0" t="n">
-        <v>6</v>
+        <v>0.2</v>
       </c>
       <c r="K19" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="M19" s="0" t="n">
-        <v>20</v>
-      </c>
       <c r="N19" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="O19" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R19" s="0" t="n">
-        <v>600</v>
-      </c>
-      <c r="S19" s="3"/>
-      <c r="T19" s="0" t="n">
+      <c r="O19" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="P19" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R19" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S19" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="T19" s="2"/>
+      <c r="U19" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U19" s="0" t="n">
+      <c r="V19" s="0" t="n">
         <v>-100</v>
       </c>
-      <c r="V19" s="0" t="s">
-        <v>69</v>
+      <c r="W19" s="0" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1860,65 +1887,68 @@
         <v>18</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>50</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I20" s="0" t="n">
-        <v>0.14</v>
+        <v>0.5</v>
       </c>
       <c r="J20" s="0" t="n">
-        <v>6</v>
+        <v>0.5</v>
       </c>
       <c r="K20" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L20" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="N20" s="0" t="n">
-        <v>50</v>
-      </c>
       <c r="O20" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="P20" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="P20" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="Q20" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="R20" s="0" t="n">
-        <v>600</v>
-      </c>
-      <c r="S20" s="3"/>
-      <c r="T20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R20" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S20" s="0" t="n">
+        <v>1400</v>
+      </c>
+      <c r="T20" s="2"/>
+      <c r="U20" s="0" t="n">
         <v>1.5</v>
       </c>
-      <c r="U20" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V20" s="0" t="s">
-        <v>71</v>
+      <c r="V20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W20" s="0" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1926,62 +1956,65 @@
         <v>19</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>80</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I21" s="0" t="n">
         <v>2.5</v>
       </c>
       <c r="J21" s="0" t="n">
-        <v>6</v>
+        <v>2.5</v>
       </c>
       <c r="K21" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L21" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="N21" s="0" t="n">
-        <v>50</v>
-      </c>
       <c r="O21" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="P21" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="P21" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="Q21" s="0" t="n">
         <v>0</v>
       </c>
       <c r="R21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S21" s="0" t="n">
         <v>200</v>
       </c>
-      <c r="S21" s="3"/>
-      <c r="T21" s="0" t="n">
+      <c r="T21" s="2"/>
+      <c r="U21" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V21" s="0" t="s">
-        <v>73</v>
+      <c r="V21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W21" s="0" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1989,62 +2022,65 @@
         <v>20</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>70</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I22" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="J22" s="0" t="n">
-        <v>6</v>
+        <v>0.5</v>
       </c>
       <c r="K22" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L22" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M22" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N22" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="O22" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P22" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q22" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R22" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="R22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S22" s="2" t="n">
         <v>1400</v>
       </c>
-      <c r="S22" s="3"/>
-      <c r="T22" s="0" t="n">
+      <c r="T22" s="2"/>
+      <c r="U22" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U22" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V22" s="0" t="s">
-        <v>76</v>
+      <c r="V22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W22" s="0" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2052,62 +2088,65 @@
         <v>21</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>75</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I23" s="0" t="n">
         <v>0.2</v>
       </c>
       <c r="J23" s="0" t="n">
-        <v>6</v>
+        <v>0.2</v>
       </c>
       <c r="K23" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L23" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M23" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N23" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="O23" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P23" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q23" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R23" s="3" t="n">
-        <v>600</v>
-      </c>
-      <c r="S23" s="3"/>
-      <c r="T23" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="R23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S23" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="T23" s="2"/>
+      <c r="U23" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U23" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V23" s="0" t="s">
-        <v>78</v>
+      <c r="V23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W23" s="0" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2115,62 +2154,65 @@
         <v>22</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>70</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I24" s="0" t="n">
         <v>0.18</v>
       </c>
       <c r="J24" s="0" t="n">
-        <v>6</v>
+        <v>0.2</v>
       </c>
       <c r="K24" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L24" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M24" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N24" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="O24" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P24" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q24" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R24" s="3" t="n">
-        <v>600</v>
-      </c>
-      <c r="S24" s="3"/>
-      <c r="T24" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="R24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S24" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="T24" s="2"/>
+      <c r="U24" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U24" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V24" s="0" t="s">
-        <v>80</v>
+      <c r="V24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W24" s="0" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2178,62 +2220,65 @@
         <v>23</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>75</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I25" s="0" t="n">
         <v>0.2</v>
       </c>
       <c r="J25" s="0" t="n">
-        <v>6</v>
+        <v>0.2</v>
       </c>
       <c r="K25" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L25" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M25" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N25" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="O25" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P25" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q25" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R25" s="3" t="n">
-        <v>600</v>
-      </c>
-      <c r="S25" s="3"/>
-      <c r="T25" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="R25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S25" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="T25" s="2"/>
+      <c r="U25" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U25" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V25" s="0" t="s">
-        <v>83</v>
+      <c r="V25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W25" s="0" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2241,62 +2286,65 @@
         <v>24</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>70</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I26" s="0" t="n">
         <v>0.18</v>
       </c>
       <c r="J26" s="0" t="n">
-        <v>6</v>
+        <v>0.2</v>
       </c>
       <c r="K26" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L26" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M26" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N26" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="O26" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P26" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q26" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R26" s="3" t="n">
-        <v>600</v>
-      </c>
-      <c r="S26" s="3"/>
-      <c r="T26" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="R26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S26" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="T26" s="2"/>
+      <c r="U26" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U26" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V26" s="0" t="s">
-        <v>85</v>
+      <c r="V26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W26" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2304,62 +2352,65 @@
         <v>25</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>65</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I27" s="0" t="n">
         <v>0.18</v>
       </c>
       <c r="J27" s="0" t="n">
-        <v>6</v>
+        <v>0.2</v>
       </c>
       <c r="K27" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L27" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M27" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N27" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="O27" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P27" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R27" s="3" t="n">
-        <v>600</v>
-      </c>
-      <c r="S27" s="3"/>
-      <c r="T27" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="R27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S27" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="T27" s="2"/>
+      <c r="U27" s="0" t="n">
         <v>1.333</v>
       </c>
-      <c r="U27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V27" s="0" t="s">
-        <v>88</v>
+      <c r="V27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W27" s="0" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2367,62 +2418,65 @@
         <v>26</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C28" s="0" t="n">
         <v>65</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I28" s="0" t="n">
         <v>0.18</v>
       </c>
       <c r="J28" s="0" t="n">
-        <v>6</v>
+        <v>0.2</v>
       </c>
       <c r="K28" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L28" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M28" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N28" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="O28" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P28" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q28" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R28" s="3" t="n">
-        <v>600</v>
-      </c>
-      <c r="S28" s="3"/>
-      <c r="T28" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="R28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S28" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="T28" s="2"/>
+      <c r="U28" s="0" t="n">
         <v>1.333</v>
       </c>
-      <c r="U28" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V28" s="0" t="s">
-        <v>90</v>
+      <c r="V28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W28" s="0" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2430,62 +2484,65 @@
         <v>27</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>65</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I29" s="0" t="n">
         <v>0.18</v>
       </c>
       <c r="J29" s="0" t="n">
-        <v>6</v>
+        <v>0.2</v>
       </c>
       <c r="K29" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L29" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M29" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N29" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="O29" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P29" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q29" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R29" s="3" t="n">
-        <v>600</v>
-      </c>
-      <c r="S29" s="3"/>
-      <c r="T29" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="R29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S29" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="T29" s="2"/>
+      <c r="U29" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U29" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V29" s="0" t="s">
-        <v>93</v>
+      <c r="V29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W29" s="0" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2493,62 +2550,65 @@
         <v>28</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>70</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I30" s="0" t="n">
         <v>0.2</v>
       </c>
       <c r="J30" s="0" t="n">
-        <v>6</v>
+        <v>0.2</v>
       </c>
       <c r="K30" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L30" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M30" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N30" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="O30" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P30" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q30" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R30" s="3" t="n">
-        <v>600</v>
-      </c>
-      <c r="S30" s="3"/>
-      <c r="T30" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="R30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S30" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="T30" s="2"/>
+      <c r="U30" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U30" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V30" s="0" t="s">
-        <v>95</v>
+      <c r="V30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W30" s="0" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2556,62 +2616,65 @@
         <v>29</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>70</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I31" s="0" t="n">
         <v>0.2</v>
       </c>
       <c r="J31" s="0" t="n">
-        <v>6</v>
+        <v>0.2</v>
       </c>
       <c r="K31" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L31" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M31" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N31" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="O31" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P31" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q31" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R31" s="3" t="n">
-        <v>600</v>
-      </c>
-      <c r="S31" s="3"/>
-      <c r="T31" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="R31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S31" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="T31" s="2"/>
+      <c r="U31" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U31" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V31" s="0" t="s">
-        <v>97</v>
+      <c r="V31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W31" s="0" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2619,62 +2682,65 @@
         <v>30</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>65</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I32" s="0" t="n">
         <v>0.14</v>
       </c>
       <c r="J32" s="0" t="n">
-        <v>6</v>
+        <v>0.14</v>
       </c>
       <c r="K32" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L32" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M32" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N32" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="O32" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P32" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q32" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R32" s="3" t="n">
-        <v>600</v>
-      </c>
-      <c r="S32" s="3"/>
-      <c r="T32" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="R32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S32" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="T32" s="2"/>
+      <c r="U32" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U32" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V32" s="0" t="s">
-        <v>99</v>
+      <c r="V32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W32" s="0" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2682,65 +2748,68 @@
         <v>31</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>70</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I33" s="0" t="n">
         <v>0.14</v>
       </c>
       <c r="J33" s="0" t="n">
-        <v>6</v>
+        <v>0.14</v>
       </c>
       <c r="K33" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L33" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M33" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N33" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="O33" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P33" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q33" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R33" s="3" t="n">
-        <v>600</v>
-      </c>
-      <c r="S33" s="3"/>
-      <c r="T33" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="R33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S33" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="T33" s="2"/>
+      <c r="U33" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U33" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V33" s="0" t="s">
-        <v>102</v>
+      <c r="V33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W33" s="0" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2748,65 +2817,68 @@
         <v>32</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C34" s="0" t="n">
         <v>70</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I34" s="0" t="n">
         <v>0.14</v>
       </c>
       <c r="J34" s="0" t="n">
-        <v>6</v>
+        <v>0.14</v>
       </c>
       <c r="K34" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L34" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M34" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N34" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="O34" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P34" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q34" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R34" s="3" t="n">
-        <v>600</v>
-      </c>
-      <c r="S34" s="3"/>
-      <c r="T34" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="R34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S34" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="T34" s="2"/>
+      <c r="U34" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U34" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V34" s="0" t="s">
-        <v>105</v>
+      <c r="V34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W34" s="0" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2814,65 +2886,68 @@
         <v>33</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>70</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I35" s="0" t="n">
         <v>0.14</v>
       </c>
       <c r="J35" s="0" t="n">
-        <v>6</v>
+        <v>0.14</v>
       </c>
       <c r="K35" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L35" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M35" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N35" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="O35" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P35" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q35" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R35" s="3" t="n">
-        <v>600</v>
-      </c>
-      <c r="S35" s="3"/>
-      <c r="T35" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="R35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S35" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="T35" s="2"/>
+      <c r="U35" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U35" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V35" s="0" t="s">
-        <v>108</v>
+      <c r="V35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W35" s="0" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2880,62 +2955,65 @@
         <v>34</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C36" s="0" t="n">
         <v>70</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I36" s="0" t="n">
         <v>0.14</v>
       </c>
       <c r="J36" s="0" t="n">
-        <v>6</v>
+        <v>0.14</v>
       </c>
       <c r="K36" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L36" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M36" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N36" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="O36" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P36" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q36" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R36" s="3" t="n">
-        <v>600</v>
-      </c>
-      <c r="S36" s="3"/>
-      <c r="T36" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="R36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S36" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="T36" s="2"/>
+      <c r="U36" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U36" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V36" s="0" t="s">
-        <v>110</v>
+      <c r="V36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W36" s="0" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2943,62 +3021,65 @@
         <v>35</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C37" s="0" t="n">
         <v>65</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I37" s="0" t="n">
         <v>0.2</v>
       </c>
       <c r="J37" s="0" t="n">
-        <v>6</v>
+        <v>0.2</v>
       </c>
       <c r="K37" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L37" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M37" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N37" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="O37" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P37" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q37" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R37" s="3" t="n">
-        <v>600</v>
-      </c>
-      <c r="S37" s="3"/>
-      <c r="T37" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="R37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S37" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="T37" s="2"/>
+      <c r="U37" s="0" t="n">
         <v>1.333</v>
       </c>
-      <c r="U37" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V37" s="0" t="s">
-        <v>112</v>
+      <c r="V37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W37" s="0" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3006,62 +3087,65 @@
         <v>36</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C38" s="0" t="n">
         <v>70</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I38" s="0" t="n">
         <v>0.14</v>
       </c>
       <c r="J38" s="0" t="n">
-        <v>6</v>
+        <v>0.14</v>
       </c>
       <c r="K38" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L38" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M38" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N38" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="O38" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P38" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q38" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R38" s="3" t="n">
-        <v>600</v>
-      </c>
-      <c r="S38" s="3"/>
-      <c r="T38" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="R38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S38" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="T38" s="2"/>
+      <c r="U38" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U38" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V38" s="0" t="s">
-        <v>114</v>
+      <c r="V38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W38" s="0" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3069,62 +3153,65 @@
         <v>37</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C39" s="0" t="n">
         <v>70</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I39" s="0" t="n">
         <v>0.2</v>
       </c>
       <c r="J39" s="0" t="n">
-        <v>6</v>
+        <v>0.2</v>
       </c>
       <c r="K39" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L39" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M39" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N39" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="O39" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P39" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q39" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R39" s="3" t="n">
-        <v>600</v>
-      </c>
-      <c r="S39" s="3"/>
-      <c r="T39" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="R39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S39" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="T39" s="2"/>
+      <c r="U39" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U39" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V39" s="0" t="s">
-        <v>116</v>
+      <c r="V39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W39" s="0" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3132,62 +3219,65 @@
         <v>38</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C40" s="0" t="n">
         <v>70</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I40" s="0" t="n">
         <v>0.2</v>
       </c>
       <c r="J40" s="0" t="n">
-        <v>6</v>
+        <v>0.2</v>
       </c>
       <c r="K40" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L40" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M40" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N40" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="O40" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P40" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q40" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R40" s="3" t="n">
-        <v>600</v>
-      </c>
-      <c r="S40" s="3"/>
-      <c r="T40" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="R40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S40" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="T40" s="2"/>
+      <c r="U40" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U40" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V40" s="0" t="s">
-        <v>118</v>
+      <c r="V40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W40" s="0" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3195,65 +3285,68 @@
         <v>39</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C41" s="0" t="n">
         <v>70</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I41" s="0" t="n">
         <v>0.14</v>
       </c>
       <c r="J41" s="0" t="n">
-        <v>6</v>
+        <v>0.14</v>
       </c>
       <c r="K41" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L41" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M41" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N41" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="O41" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P41" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q41" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R41" s="3" t="n">
-        <v>600</v>
-      </c>
-      <c r="S41" s="3"/>
-      <c r="T41" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="R41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S41" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="T41" s="2"/>
+      <c r="U41" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U41" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V41" s="0" t="s">
-        <v>120</v>
+      <c r="V41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W41" s="0" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3261,62 +3354,65 @@
         <v>40</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C42" s="0" t="n">
         <v>65</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="I42" s="0" t="n">
         <v>0.18</v>
       </c>
       <c r="J42" s="0" t="n">
-        <v>6</v>
+        <v>0.2</v>
       </c>
       <c r="K42" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L42" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M42" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N42" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="O42" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P42" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q42" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R42" s="3" t="n">
-        <v>600</v>
-      </c>
-      <c r="S42" s="3"/>
-      <c r="T42" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="R42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S42" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="T42" s="2"/>
+      <c r="U42" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U42" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V42" s="0" t="s">
-        <v>123</v>
+      <c r="V42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W42" s="0" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3324,65 +3420,68 @@
         <v>41</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C43" s="0" t="n">
         <v>70</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I43" s="0" t="n">
         <v>0.14</v>
       </c>
       <c r="J43" s="0" t="n">
-        <v>6</v>
+        <v>0.14</v>
       </c>
       <c r="K43" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L43" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M43" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N43" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="O43" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P43" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q43" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R43" s="3" t="n">
-        <v>600</v>
-      </c>
-      <c r="S43" s="3"/>
-      <c r="T43" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="R43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S43" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="T43" s="2"/>
+      <c r="U43" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U43" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V43" s="0" t="s">
-        <v>126</v>
+      <c r="V43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W43" s="0" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3390,62 +3489,65 @@
         <v>42</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C44" s="0" t="n">
         <v>65</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I44" s="0" t="n">
         <v>0.2</v>
       </c>
       <c r="J44" s="0" t="n">
-        <v>6</v>
+        <v>0.2</v>
       </c>
       <c r="K44" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L44" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M44" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N44" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="O44" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P44" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q44" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R44" s="3" t="n">
-        <v>600</v>
-      </c>
-      <c r="S44" s="3"/>
-      <c r="T44" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="R44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S44" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="T44" s="2"/>
+      <c r="U44" s="0" t="n">
         <v>1.333</v>
       </c>
-      <c r="U44" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V44" s="0" t="s">
-        <v>128</v>
+      <c r="V44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W44" s="0" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3453,62 +3555,65 @@
         <v>43</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C45" s="0" t="n">
         <v>70</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I45" s="0" t="n">
         <v>0.14</v>
       </c>
       <c r="J45" s="0" t="n">
-        <v>6</v>
+        <v>0.14</v>
       </c>
       <c r="K45" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L45" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M45" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N45" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="O45" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P45" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q45" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R45" s="3" t="n">
-        <v>600</v>
-      </c>
-      <c r="S45" s="3"/>
-      <c r="T45" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="R45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S45" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="T45" s="2"/>
+      <c r="U45" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U45" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V45" s="0" t="s">
-        <v>130</v>
+      <c r="V45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W45" s="0" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3516,65 +3621,68 @@
         <v>44</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C46" s="0" t="n">
         <v>70</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I46" s="0" t="n">
         <v>0.14</v>
       </c>
       <c r="J46" s="0" t="n">
-        <v>6</v>
+        <v>0.14</v>
       </c>
       <c r="K46" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L46" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M46" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N46" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="O46" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P46" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q46" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R46" s="3" t="n">
-        <v>600</v>
-      </c>
-      <c r="S46" s="3"/>
-      <c r="T46" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="R46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S46" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="T46" s="2"/>
+      <c r="U46" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U46" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V46" s="0" t="s">
-        <v>132</v>
+      <c r="V46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W46" s="0" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3582,62 +3690,65 @@
         <v>45</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C47" s="0" t="n">
         <v>70</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I47" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="J47" s="0" t="n">
-        <v>6</v>
+        <v>0.2</v>
       </c>
       <c r="K47" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L47" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M47" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N47" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="O47" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P47" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q47" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R47" s="3" t="n">
-        <v>600</v>
-      </c>
-      <c r="S47" s="3"/>
-      <c r="T47" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="R47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S47" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="T47" s="2"/>
+      <c r="U47" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U47" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V47" s="0" t="s">
-        <v>134</v>
+      <c r="V47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W47" s="0" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3645,62 +3756,65 @@
         <v>46</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C48" s="0" t="n">
         <v>65</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I48" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="J48" s="0" t="n">
-        <v>6</v>
+        <v>0.2</v>
       </c>
       <c r="K48" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L48" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M48" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N48" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="O48" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P48" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q48" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R48" s="3" t="n">
-        <v>600</v>
-      </c>
-      <c r="S48" s="3"/>
-      <c r="T48" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="R48" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S48" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="T48" s="2"/>
+      <c r="U48" s="0" t="n">
         <v>1.333</v>
       </c>
-      <c r="U48" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V48" s="0" t="s">
-        <v>136</v>
+      <c r="V48" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W48" s="0" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3708,65 +3822,68 @@
         <v>47</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C49" s="0" t="n">
         <v>70</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="I49" s="0" t="n">
         <v>0.14</v>
       </c>
       <c r="J49" s="0" t="n">
-        <v>6</v>
+        <v>0.14</v>
       </c>
       <c r="K49" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L49" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M49" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N49" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="O49" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P49" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q49" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R49" s="3" t="n">
-        <v>600</v>
-      </c>
-      <c r="S49" s="3"/>
-      <c r="T49" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="R49" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S49" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="T49" s="2"/>
+      <c r="U49" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U49" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V49" s="0" t="s">
-        <v>139</v>
+      <c r="V49" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W49" s="0" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3774,65 +3891,68 @@
         <v>48</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C50" s="0" t="n">
         <v>70</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="I50" s="0" t="n">
         <v>0.14</v>
       </c>
       <c r="J50" s="0" t="n">
-        <v>6</v>
+        <v>0.14</v>
       </c>
       <c r="K50" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L50" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M50" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N50" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="O50" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P50" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q50" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R50" s="3" t="n">
-        <v>600</v>
-      </c>
-      <c r="S50" s="3"/>
-      <c r="T50" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="R50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S50" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="T50" s="2"/>
+      <c r="U50" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U50" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V50" s="0" t="s">
-        <v>141</v>
+      <c r="V50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W50" s="0" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3840,62 +3960,65 @@
         <v>49</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C51" s="0" t="n">
         <v>65</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I51" s="0" t="n">
         <v>2.5</v>
       </c>
       <c r="J51" s="0" t="n">
-        <v>6</v>
+        <v>2.5</v>
       </c>
       <c r="K51" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L51" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M51" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N51" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="O51" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P51" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q51" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R51" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="R51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S51" s="2" t="n">
         <v>200</v>
       </c>
-      <c r="S51" s="3"/>
-      <c r="T51" s="0" t="n">
+      <c r="T51" s="2"/>
+      <c r="U51" s="0" t="n">
         <v>1.333</v>
       </c>
-      <c r="U51" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V51" s="0" t="s">
-        <v>143</v>
+      <c r="V51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W51" s="0" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3903,62 +4026,65 @@
         <v>50</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C52" s="0" t="n">
         <v>65</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="I52" s="0" t="n">
         <v>0.14</v>
       </c>
       <c r="J52" s="0" t="n">
-        <v>6</v>
+        <v>0.14</v>
       </c>
       <c r="K52" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L52" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M52" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N52" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="O52" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P52" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q52" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R52" s="3" t="n">
-        <v>600</v>
-      </c>
-      <c r="S52" s="3"/>
-      <c r="T52" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="R52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S52" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="T52" s="2"/>
+      <c r="U52" s="0" t="n">
         <v>1.333</v>
       </c>
-      <c r="U52" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V52" s="0" t="s">
-        <v>146</v>
+      <c r="V52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W52" s="0" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3966,65 +4092,68 @@
         <v>51</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C53" s="0" t="n">
         <v>65</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="I53" s="0" t="n">
         <v>0.14</v>
       </c>
       <c r="J53" s="0" t="n">
-        <v>6</v>
+        <v>0.14</v>
       </c>
       <c r="K53" s="0" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="L53" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M53" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N53" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="O53" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P53" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q53" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R53" s="3" t="n">
-        <v>600</v>
-      </c>
-      <c r="S53" s="3"/>
-      <c r="T53" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="R53" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S53" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="T53" s="2"/>
+      <c r="U53" s="0" t="n">
         <v>1.333</v>
       </c>
-      <c r="U53" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V53" s="0" t="s">
-        <v>149</v>
+      <c r="V53" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W53" s="0" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update: fix db and boiling plan
</commit_message>
<xml_diff>
--- a/app/data/static/params/mascarpone.xlsx
+++ b/app/data/static/params/mascarpone.xlsx
@@ -608,8 +608,8 @@
   </sheetPr>
   <dimension ref="A1:W53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H22" activeCellId="0" sqref="H22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P21" activeCellId="0" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -740,7 +740,9 @@
       <c r="S2" s="0" t="n">
         <v>600</v>
       </c>
-      <c r="T2" s="2"/>
+      <c r="T2" s="2" t="n">
+        <v>600</v>
+      </c>
       <c r="U2" s="0" t="n">
         <v>1</v>
       </c>
@@ -806,7 +808,9 @@
       <c r="S3" s="0" t="n">
         <v>600</v>
       </c>
-      <c r="T3" s="2"/>
+      <c r="T3" s="2" t="n">
+        <v>600</v>
+      </c>
       <c r="U3" s="0" t="n">
         <v>1</v>
       </c>
@@ -872,7 +876,9 @@
       <c r="S4" s="0" t="n">
         <v>1400</v>
       </c>
-      <c r="T4" s="2"/>
+      <c r="T4" s="2" t="n">
+        <v>600</v>
+      </c>
       <c r="U4" s="0" t="n">
         <v>1</v>
       </c>
@@ -938,7 +944,9 @@
       <c r="S5" s="0" t="n">
         <v>600</v>
       </c>
-      <c r="T5" s="2"/>
+      <c r="T5" s="2" t="n">
+        <v>600</v>
+      </c>
       <c r="U5" s="0" t="n">
         <v>1</v>
       </c>
@@ -1007,7 +1015,9 @@
       <c r="S6" s="0" t="n">
         <v>600</v>
       </c>
-      <c r="T6" s="2"/>
+      <c r="T6" s="2" t="n">
+        <v>600</v>
+      </c>
       <c r="U6" s="0" t="n">
         <v>1.5</v>
       </c>
@@ -1073,7 +1083,9 @@
       <c r="S7" s="0" t="n">
         <v>600</v>
       </c>
-      <c r="T7" s="2"/>
+      <c r="T7" s="2" t="n">
+        <v>600</v>
+      </c>
       <c r="U7" s="0" t="n">
         <v>1</v>
       </c>
@@ -1139,7 +1151,9 @@
       <c r="S8" s="0" t="n">
         <v>600</v>
       </c>
-      <c r="T8" s="2"/>
+      <c r="T8" s="2" t="n">
+        <v>600</v>
+      </c>
       <c r="U8" s="0" t="n">
         <v>1</v>
       </c>
@@ -1205,7 +1219,9 @@
       <c r="S9" s="0" t="n">
         <v>1400</v>
       </c>
-      <c r="T9" s="2"/>
+      <c r="T9" s="2" t="n">
+        <v>600</v>
+      </c>
       <c r="U9" s="0" t="n">
         <v>1</v>
       </c>
@@ -1274,7 +1290,9 @@
       <c r="S10" s="0" t="n">
         <v>600</v>
       </c>
-      <c r="T10" s="2"/>
+      <c r="T10" s="2" t="n">
+        <v>600</v>
+      </c>
       <c r="U10" s="0" t="n">
         <v>1.5</v>
       </c>
@@ -1340,7 +1358,9 @@
       <c r="S11" s="4" t="n">
         <v>1400</v>
       </c>
-      <c r="T11" s="2"/>
+      <c r="T11" s="2" t="n">
+        <v>300</v>
+      </c>
       <c r="U11" s="0" t="n">
         <v>1</v>
       </c>
@@ -1406,7 +1426,9 @@
       <c r="S12" s="0" t="n">
         <v>600</v>
       </c>
-      <c r="T12" s="2"/>
+      <c r="T12" s="2" t="n">
+        <v>300</v>
+      </c>
       <c r="U12" s="0" t="n">
         <v>1</v>
       </c>
@@ -1472,7 +1494,9 @@
       <c r="S13" s="0" t="n">
         <v>600</v>
       </c>
-      <c r="T13" s="2"/>
+      <c r="T13" s="2" t="n">
+        <v>300</v>
+      </c>
       <c r="U13" s="0" t="n">
         <v>1</v>
       </c>
@@ -1538,7 +1562,9 @@
       <c r="S14" s="0" t="n">
         <v>600</v>
       </c>
-      <c r="T14" s="2"/>
+      <c r="T14" s="2" t="n">
+        <v>600</v>
+      </c>
       <c r="U14" s="0" t="n">
         <v>1</v>
       </c>
@@ -1604,7 +1630,9 @@
       <c r="S15" s="0" t="n">
         <v>600</v>
       </c>
-      <c r="T15" s="2"/>
+      <c r="T15" s="2" t="n">
+        <v>600</v>
+      </c>
       <c r="U15" s="0" t="n">
         <v>1</v>
       </c>
@@ -1673,7 +1701,9 @@
       <c r="S16" s="0" t="n">
         <v>600</v>
       </c>
-      <c r="T16" s="2"/>
+      <c r="T16" s="2" t="n">
+        <v>600</v>
+      </c>
       <c r="U16" s="0" t="n">
         <v>1.5</v>
       </c>
@@ -1739,7 +1769,9 @@
       <c r="S17" s="0" t="n">
         <v>1400</v>
       </c>
-      <c r="T17" s="2"/>
+      <c r="T17" s="2" t="n">
+        <v>300</v>
+      </c>
       <c r="U17" s="0" t="n">
         <v>1</v>
       </c>
@@ -1805,7 +1837,9 @@
       <c r="S18" s="0" t="n">
         <v>600</v>
       </c>
-      <c r="T18" s="2"/>
+      <c r="T18" s="2" t="n">
+        <v>600</v>
+      </c>
       <c r="U18" s="0" t="n">
         <v>1</v>
       </c>
@@ -1871,7 +1905,9 @@
       <c r="S19" s="0" t="n">
         <v>600</v>
       </c>
-      <c r="T19" s="2"/>
+      <c r="T19" s="2" t="n">
+        <v>300</v>
+      </c>
       <c r="U19" s="0" t="n">
         <v>1</v>
       </c>
@@ -1940,7 +1976,9 @@
       <c r="S20" s="0" t="n">
         <v>1400</v>
       </c>
-      <c r="T20" s="2"/>
+      <c r="T20" s="2" t="n">
+        <v>600</v>
+      </c>
       <c r="U20" s="0" t="n">
         <v>1.5</v>
       </c>
@@ -2006,7 +2044,9 @@
       <c r="S21" s="0" t="n">
         <v>200</v>
       </c>
-      <c r="T21" s="2"/>
+      <c r="T21" s="2" t="n">
+        <v>600</v>
+      </c>
       <c r="U21" s="0" t="n">
         <v>1</v>
       </c>
@@ -2072,7 +2112,9 @@
       <c r="S22" s="2" t="n">
         <v>1400</v>
       </c>
-      <c r="T22" s="2"/>
+      <c r="T22" s="2" t="n">
+        <v>370</v>
+      </c>
       <c r="U22" s="0" t="n">
         <v>1</v>
       </c>
@@ -2136,9 +2178,11 @@
         <v>0</v>
       </c>
       <c r="S23" s="2" t="n">
-        <v>600</v>
-      </c>
-      <c r="T23" s="2"/>
+        <v>800</v>
+      </c>
+      <c r="T23" s="2" t="n">
+        <v>370</v>
+      </c>
       <c r="U23" s="0" t="n">
         <v>1</v>
       </c>
@@ -2202,9 +2246,11 @@
         <v>0</v>
       </c>
       <c r="S24" s="2" t="n">
-        <v>600</v>
-      </c>
-      <c r="T24" s="2"/>
+        <v>800</v>
+      </c>
+      <c r="T24" s="2" t="n">
+        <v>370</v>
+      </c>
       <c r="U24" s="0" t="n">
         <v>1</v>
       </c>
@@ -2268,9 +2314,11 @@
         <v>0</v>
       </c>
       <c r="S25" s="2" t="n">
-        <v>600</v>
-      </c>
-      <c r="T25" s="2"/>
+        <v>800</v>
+      </c>
+      <c r="T25" s="2" t="n">
+        <v>370</v>
+      </c>
       <c r="U25" s="0" t="n">
         <v>1</v>
       </c>
@@ -2334,9 +2382,11 @@
         <v>0</v>
       </c>
       <c r="S26" s="2" t="n">
-        <v>600</v>
-      </c>
-      <c r="T26" s="2"/>
+        <v>800</v>
+      </c>
+      <c r="T26" s="2" t="n">
+        <v>370</v>
+      </c>
       <c r="U26" s="0" t="n">
         <v>1</v>
       </c>
@@ -2400,11 +2450,13 @@
         <v>0</v>
       </c>
       <c r="S27" s="2" t="n">
-        <v>600</v>
-      </c>
-      <c r="T27" s="2"/>
+        <v>800</v>
+      </c>
+      <c r="T27" s="2" t="n">
+        <v>370</v>
+      </c>
       <c r="U27" s="0" t="n">
-        <v>1.333</v>
+        <v>1.42</v>
       </c>
       <c r="V27" s="0" t="n">
         <v>0</v>
@@ -2466,11 +2518,13 @@
         <v>0</v>
       </c>
       <c r="S28" s="2" t="n">
-        <v>600</v>
-      </c>
-      <c r="T28" s="2"/>
+        <v>800</v>
+      </c>
+      <c r="T28" s="2" t="n">
+        <v>370</v>
+      </c>
       <c r="U28" s="0" t="n">
-        <v>1.333</v>
+        <v>1.42</v>
       </c>
       <c r="V28" s="0" t="n">
         <v>0</v>
@@ -2532,9 +2586,11 @@
         <v>0</v>
       </c>
       <c r="S29" s="2" t="n">
-        <v>600</v>
-      </c>
-      <c r="T29" s="2"/>
+        <v>800</v>
+      </c>
+      <c r="T29" s="2" t="n">
+        <v>370</v>
+      </c>
       <c r="U29" s="0" t="n">
         <v>1</v>
       </c>
@@ -2598,9 +2654,11 @@
         <v>0</v>
       </c>
       <c r="S30" s="2" t="n">
-        <v>600</v>
-      </c>
-      <c r="T30" s="2"/>
+        <v>800</v>
+      </c>
+      <c r="T30" s="2" t="n">
+        <v>370</v>
+      </c>
       <c r="U30" s="0" t="n">
         <v>1</v>
       </c>
@@ -2664,9 +2722,11 @@
         <v>0</v>
       </c>
       <c r="S31" s="2" t="n">
-        <v>600</v>
-      </c>
-      <c r="T31" s="2"/>
+        <v>800</v>
+      </c>
+      <c r="T31" s="2" t="n">
+        <v>370</v>
+      </c>
       <c r="U31" s="0" t="n">
         <v>1</v>
       </c>
@@ -2730,9 +2790,11 @@
         <v>0</v>
       </c>
       <c r="S32" s="2" t="n">
-        <v>600</v>
-      </c>
-      <c r="T32" s="2"/>
+        <v>700</v>
+      </c>
+      <c r="T32" s="2" t="n">
+        <v>370</v>
+      </c>
       <c r="U32" s="0" t="n">
         <v>1</v>
       </c>
@@ -2799,11 +2861,13 @@
         <v>0</v>
       </c>
       <c r="S33" s="2" t="n">
-        <v>600</v>
-      </c>
-      <c r="T33" s="2"/>
+        <v>700</v>
+      </c>
+      <c r="T33" s="2" t="n">
+        <v>370</v>
+      </c>
       <c r="U33" s="0" t="n">
-        <v>1</v>
+        <v>1.07</v>
       </c>
       <c r="V33" s="0" t="n">
         <v>0</v>
@@ -2868,11 +2932,13 @@
         <v>0</v>
       </c>
       <c r="S34" s="2" t="n">
-        <v>600</v>
-      </c>
-      <c r="T34" s="2"/>
+        <v>700</v>
+      </c>
+      <c r="T34" s="2" t="n">
+        <v>370</v>
+      </c>
       <c r="U34" s="0" t="n">
-        <v>1</v>
+        <v>1.07</v>
       </c>
       <c r="V34" s="0" t="n">
         <v>0</v>
@@ -2937,11 +3003,13 @@
         <v>0</v>
       </c>
       <c r="S35" s="2" t="n">
-        <v>600</v>
-      </c>
-      <c r="T35" s="2"/>
+        <v>700</v>
+      </c>
+      <c r="T35" s="2" t="n">
+        <v>370</v>
+      </c>
       <c r="U35" s="0" t="n">
-        <v>1</v>
+        <v>1.07</v>
       </c>
       <c r="V35" s="0" t="n">
         <v>0</v>
@@ -3003,9 +3071,11 @@
         <v>0</v>
       </c>
       <c r="S36" s="2" t="n">
-        <v>600</v>
-      </c>
-      <c r="T36" s="2"/>
+        <v>700</v>
+      </c>
+      <c r="T36" s="2" t="n">
+        <v>370</v>
+      </c>
       <c r="U36" s="0" t="n">
         <v>1</v>
       </c>
@@ -3069,11 +3139,13 @@
         <v>0</v>
       </c>
       <c r="S37" s="2" t="n">
-        <v>600</v>
-      </c>
-      <c r="T37" s="2"/>
+        <v>800</v>
+      </c>
+      <c r="T37" s="2" t="n">
+        <v>370</v>
+      </c>
       <c r="U37" s="0" t="n">
-        <v>1.333</v>
+        <v>1.42</v>
       </c>
       <c r="V37" s="0" t="n">
         <v>0</v>
@@ -3135,9 +3207,11 @@
         <v>0</v>
       </c>
       <c r="S38" s="2" t="n">
-        <v>600</v>
-      </c>
-      <c r="T38" s="2"/>
+        <v>700</v>
+      </c>
+      <c r="T38" s="2" t="n">
+        <v>370</v>
+      </c>
       <c r="U38" s="0" t="n">
         <v>1</v>
       </c>
@@ -3201,9 +3275,11 @@
         <v>0</v>
       </c>
       <c r="S39" s="2" t="n">
-        <v>600</v>
-      </c>
-      <c r="T39" s="2"/>
+        <v>800</v>
+      </c>
+      <c r="T39" s="2" t="n">
+        <v>370</v>
+      </c>
       <c r="U39" s="0" t="n">
         <v>1</v>
       </c>
@@ -3267,9 +3343,11 @@
         <v>0</v>
       </c>
       <c r="S40" s="2" t="n">
-        <v>600</v>
-      </c>
-      <c r="T40" s="2"/>
+        <v>800</v>
+      </c>
+      <c r="T40" s="2" t="n">
+        <v>370</v>
+      </c>
       <c r="U40" s="0" t="n">
         <v>1</v>
       </c>
@@ -3336,11 +3414,13 @@
         <v>0</v>
       </c>
       <c r="S41" s="2" t="n">
-        <v>600</v>
-      </c>
-      <c r="T41" s="2"/>
+        <v>700</v>
+      </c>
+      <c r="T41" s="2" t="n">
+        <v>370</v>
+      </c>
       <c r="U41" s="0" t="n">
-        <v>1</v>
+        <v>1.07</v>
       </c>
       <c r="V41" s="0" t="n">
         <v>0</v>
@@ -3402,9 +3482,11 @@
         <v>0</v>
       </c>
       <c r="S42" s="2" t="n">
-        <v>600</v>
-      </c>
-      <c r="T42" s="2"/>
+        <v>800</v>
+      </c>
+      <c r="T42" s="2" t="n">
+        <v>370</v>
+      </c>
       <c r="U42" s="0" t="n">
         <v>1</v>
       </c>
@@ -3471,11 +3553,13 @@
         <v>0</v>
       </c>
       <c r="S43" s="2" t="n">
-        <v>600</v>
-      </c>
-      <c r="T43" s="2"/>
+        <v>700</v>
+      </c>
+      <c r="T43" s="2" t="n">
+        <v>370</v>
+      </c>
       <c r="U43" s="0" t="n">
-        <v>1</v>
+        <v>1.07</v>
       </c>
       <c r="V43" s="0" t="n">
         <v>0</v>
@@ -3537,11 +3621,13 @@
         <v>0</v>
       </c>
       <c r="S44" s="2" t="n">
-        <v>600</v>
-      </c>
-      <c r="T44" s="2"/>
+        <v>800</v>
+      </c>
+      <c r="T44" s="2" t="n">
+        <v>370</v>
+      </c>
       <c r="U44" s="0" t="n">
-        <v>1.333</v>
+        <v>1.42</v>
       </c>
       <c r="V44" s="0" t="n">
         <v>0</v>
@@ -3603,9 +3689,11 @@
         <v>0</v>
       </c>
       <c r="S45" s="2" t="n">
-        <v>600</v>
-      </c>
-      <c r="T45" s="2"/>
+        <v>700</v>
+      </c>
+      <c r="T45" s="2" t="n">
+        <v>370</v>
+      </c>
       <c r="U45" s="0" t="n">
         <v>1</v>
       </c>
@@ -3672,11 +3760,13 @@
         <v>0</v>
       </c>
       <c r="S46" s="2" t="n">
-        <v>600</v>
-      </c>
-      <c r="T46" s="2"/>
+        <v>700</v>
+      </c>
+      <c r="T46" s="2" t="n">
+        <v>370</v>
+      </c>
       <c r="U46" s="0" t="n">
-        <v>1</v>
+        <v>1.07</v>
       </c>
       <c r="V46" s="0" t="n">
         <v>0</v>
@@ -3738,9 +3828,11 @@
         <v>0</v>
       </c>
       <c r="S47" s="2" t="n">
-        <v>600</v>
-      </c>
-      <c r="T47" s="2"/>
+        <v>800</v>
+      </c>
+      <c r="T47" s="2" t="n">
+        <v>370</v>
+      </c>
       <c r="U47" s="0" t="n">
         <v>1</v>
       </c>
@@ -3804,11 +3896,13 @@
         <v>0</v>
       </c>
       <c r="S48" s="2" t="n">
-        <v>600</v>
-      </c>
-      <c r="T48" s="2"/>
+        <v>800</v>
+      </c>
+      <c r="T48" s="2" t="n">
+        <v>370</v>
+      </c>
       <c r="U48" s="0" t="n">
-        <v>1.333</v>
+        <v>1.42</v>
       </c>
       <c r="V48" s="0" t="n">
         <v>0</v>
@@ -3873,11 +3967,13 @@
         <v>0</v>
       </c>
       <c r="S49" s="2" t="n">
-        <v>600</v>
-      </c>
-      <c r="T49" s="2"/>
+        <v>700</v>
+      </c>
+      <c r="T49" s="2" t="n">
+        <v>370</v>
+      </c>
       <c r="U49" s="0" t="n">
-        <v>1</v>
+        <v>1.07</v>
       </c>
       <c r="V49" s="0" t="n">
         <v>0</v>
@@ -3942,11 +4038,13 @@
         <v>0</v>
       </c>
       <c r="S50" s="2" t="n">
-        <v>600</v>
-      </c>
-      <c r="T50" s="2"/>
+        <v>700</v>
+      </c>
+      <c r="T50" s="2" t="n">
+        <v>370</v>
+      </c>
       <c r="U50" s="0" t="n">
-        <v>1</v>
+        <v>1.07</v>
       </c>
       <c r="V50" s="0" t="n">
         <v>0</v>
@@ -4010,9 +4108,11 @@
       <c r="S51" s="2" t="n">
         <v>200</v>
       </c>
-      <c r="T51" s="2"/>
+      <c r="T51" s="2" t="n">
+        <v>370</v>
+      </c>
       <c r="U51" s="0" t="n">
-        <v>1.333</v>
+        <v>1.42</v>
       </c>
       <c r="V51" s="0" t="n">
         <v>0</v>
@@ -4074,11 +4174,13 @@
         <v>0</v>
       </c>
       <c r="S52" s="2" t="n">
-        <v>600</v>
-      </c>
-      <c r="T52" s="2"/>
+        <v>700</v>
+      </c>
+      <c r="T52" s="2" t="n">
+        <v>370</v>
+      </c>
       <c r="U52" s="0" t="n">
-        <v>1.333</v>
+        <v>1.42</v>
       </c>
       <c r="V52" s="0" t="n">
         <v>0</v>
@@ -4143,11 +4245,13 @@
         <v>0</v>
       </c>
       <c r="S53" s="2" t="n">
-        <v>600</v>
-      </c>
-      <c r="T53" s="2"/>
+        <v>700</v>
+      </c>
+      <c r="T53" s="2" t="n">
+        <v>370</v>
+      </c>
       <c r="U53" s="0" t="n">
-        <v>1.333</v>
+        <v>1.42</v>
       </c>
       <c r="V53" s="0" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Fix: change boiling plan reading
</commit_message>
<xml_diff>
--- a/app/data/static/params/mascarpone.xlsx
+++ b/app/data/static/params/mascarpone.xlsx
@@ -513,7 +513,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -524,6 +524,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD4EA6B"/>
+        <bgColor rgb="FFCCFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -568,7 +574,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -589,6 +595,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -598,6 +616,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFD4EA6B"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -608,8 +686,8 @@
   </sheetPr>
   <dimension ref="A1:W53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O20" activeCellId="0" sqref="O20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S53" activeCellId="0" sqref="S53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1722,7 +1800,7 @@
         <v>64</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>23</v>
@@ -2397,139 +2475,139 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="n">
+    <row r="27" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5" t="n">
         <v>25</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C27" s="0" t="n">
+      <c r="C27" s="6" t="n">
         <v>65</v>
       </c>
-      <c r="D27" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="F27" s="0" t="s">
+      <c r="D27" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="G27" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="H27" s="0" t="s">
+      <c r="G27" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H27" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="I27" s="0" t="n">
+      <c r="I27" s="6" t="n">
         <v>0.18</v>
       </c>
-      <c r="J27" s="0" t="n">
+      <c r="J27" s="6" t="n">
         <v>0.2</v>
       </c>
-      <c r="K27" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="L27" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="M27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N27" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="O27" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="P27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q27" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="R27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S27" s="2" t="n">
+      <c r="K27" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="L27" s="6" t="n">
+        <v>50</v>
+      </c>
+      <c r="M27" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N27" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="O27" s="6" t="n">
+        <v>60</v>
+      </c>
+      <c r="P27" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="R27" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S27" s="6" t="n">
         <v>800</v>
       </c>
-      <c r="T27" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="U27" s="0" t="n">
+      <c r="T27" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="U27" s="6" t="n">
         <v>0.525</v>
       </c>
-      <c r="V27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="W27" s="0" t="s">
+      <c r="V27" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W27" s="6" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="n">
+    <row r="28" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5" t="n">
         <v>26</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="C28" s="0" t="n">
+      <c r="C28" s="6" t="n">
         <v>65</v>
       </c>
-      <c r="D28" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="F28" s="0" t="s">
+      <c r="D28" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="G28" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="H28" s="0" t="s">
+      <c r="G28" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H28" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I28" s="0" t="n">
+      <c r="I28" s="6" t="n">
         <v>0.18</v>
       </c>
-      <c r="J28" s="0" t="n">
+      <c r="J28" s="6" t="n">
         <v>0.2</v>
       </c>
-      <c r="K28" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="L28" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="M28" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N28" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="O28" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="P28" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q28" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="R28" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S28" s="2" t="n">
+      <c r="K28" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="L28" s="6" t="n">
+        <v>50</v>
+      </c>
+      <c r="M28" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N28" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="O28" s="6" t="n">
+        <v>60</v>
+      </c>
+      <c r="P28" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="R28" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S28" s="6" t="n">
         <v>800</v>
       </c>
-      <c r="T28" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="U28" s="0" t="n">
+      <c r="T28" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="U28" s="6" t="n">
         <v>0.525</v>
       </c>
-      <c r="V28" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="W28" s="0" t="s">
+      <c r="V28" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W28" s="6" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3086,71 +3164,71 @@
         <v>111</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="n">
+    <row r="37" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="C37" s="0" t="n">
+      <c r="C37" s="6" t="n">
         <v>65</v>
       </c>
-      <c r="D37" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="F37" s="0" t="s">
+      <c r="D37" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F37" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="G37" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="H37" s="0" t="s">
+      <c r="G37" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H37" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I37" s="0" t="n">
+      <c r="I37" s="6" t="n">
         <v>0.2</v>
       </c>
-      <c r="J37" s="0" t="n">
+      <c r="J37" s="6" t="n">
         <v>0.2</v>
       </c>
-      <c r="K37" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="L37" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="M37" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N37" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="O37" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="P37" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q37" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="R37" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S37" s="2" t="n">
+      <c r="K37" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="L37" s="6" t="n">
+        <v>50</v>
+      </c>
+      <c r="M37" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N37" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="O37" s="6" t="n">
+        <v>60</v>
+      </c>
+      <c r="P37" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="R37" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S37" s="6" t="n">
         <v>800</v>
       </c>
-      <c r="T37" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="U37" s="0" t="n">
+      <c r="T37" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="U37" s="6" t="n">
         <v>0.525</v>
       </c>
-      <c r="V37" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="W37" s="0" t="s">
+      <c r="V37" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W37" s="6" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3568,71 +3646,71 @@
         <v>127</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="n">
+    <row r="44" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="5" t="n">
         <v>42</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="B44" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="C44" s="0" t="n">
+      <c r="C44" s="6" t="n">
         <v>65</v>
       </c>
-      <c r="D44" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="F44" s="0" t="s">
+      <c r="D44" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F44" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="G44" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="H44" s="0" t="s">
+      <c r="G44" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H44" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I44" s="0" t="n">
+      <c r="I44" s="6" t="n">
         <v>0.2</v>
       </c>
-      <c r="J44" s="0" t="n">
+      <c r="J44" s="6" t="n">
         <v>0.2</v>
       </c>
-      <c r="K44" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="L44" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="M44" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N44" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="O44" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="P44" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q44" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="R44" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S44" s="2" t="n">
+      <c r="K44" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="L44" s="6" t="n">
+        <v>50</v>
+      </c>
+      <c r="M44" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N44" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="O44" s="6" t="n">
+        <v>60</v>
+      </c>
+      <c r="P44" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="R44" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S44" s="6" t="n">
         <v>800</v>
       </c>
-      <c r="T44" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="U44" s="0" t="n">
+      <c r="T44" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="U44" s="6" t="n">
         <v>0.525</v>
       </c>
-      <c r="V44" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="W44" s="0" t="s">
+      <c r="V44" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W44" s="6" t="s">
         <v>129</v>
       </c>
     </row>
@@ -3843,71 +3921,71 @@
         <v>135</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="n">
+    <row r="48" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="5" t="n">
         <v>46</v>
       </c>
-      <c r="B48" s="0" t="s">
+      <c r="B48" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C48" s="0" t="n">
+      <c r="C48" s="6" t="n">
         <v>65</v>
       </c>
-      <c r="D48" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="F48" s="0" t="s">
+      <c r="D48" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F48" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="G48" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="H48" s="0" t="s">
+      <c r="G48" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H48" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I48" s="0" t="n">
+      <c r="I48" s="6" t="n">
         <v>0.25</v>
       </c>
-      <c r="J48" s="0" t="n">
+      <c r="J48" s="6" t="n">
         <v>0.2</v>
       </c>
-      <c r="K48" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="L48" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="M48" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N48" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="O48" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="P48" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q48" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="R48" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S48" s="2" t="n">
+      <c r="K48" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="L48" s="6" t="n">
+        <v>50</v>
+      </c>
+      <c r="M48" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N48" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="O48" s="6" t="n">
+        <v>60</v>
+      </c>
+      <c r="P48" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q48" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="R48" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S48" s="6" t="n">
         <v>800</v>
       </c>
-      <c r="T48" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="U48" s="0" t="n">
+      <c r="T48" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="U48" s="6" t="n">
         <v>0.525</v>
       </c>
-      <c r="V48" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="W48" s="0" t="s">
+      <c r="V48" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W48" s="6" t="s">
         <v>137</v>
       </c>
     </row>
@@ -4100,7 +4178,7 @@
         <v>0</v>
       </c>
       <c r="Q51" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="R51" s="0" t="n">
         <v>0</v>
@@ -4121,142 +4199,142 @@
         <v>144</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="B52" s="0" t="s">
+    <row r="52" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="5" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="C52" s="0" t="n">
+      <c r="C52" s="6" t="n">
         <v>65</v>
       </c>
-      <c r="D52" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="F52" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="G52" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="H52" s="0" t="s">
+      <c r="D52" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H52" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="I52" s="0" t="n">
+      <c r="I52" s="6" t="n">
         <v>0.14</v>
       </c>
-      <c r="J52" s="0" t="n">
+      <c r="J52" s="6" t="n">
         <v>0.14</v>
       </c>
-      <c r="K52" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="L52" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="M52" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N52" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="O52" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="P52" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q52" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="R52" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S52" s="2" t="n">
+      <c r="K52" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="L52" s="6" t="n">
+        <v>50</v>
+      </c>
+      <c r="M52" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N52" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="O52" s="6" t="n">
+        <v>60</v>
+      </c>
+      <c r="P52" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q52" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="R52" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S52" s="6" t="n">
         <v>700</v>
       </c>
-      <c r="T52" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="U52" s="0" t="n">
+      <c r="T52" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="U52" s="6" t="n">
         <v>0.525</v>
       </c>
-      <c r="V52" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="W52" s="0" t="s">
+      <c r="V52" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W52" s="6" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="n">
+    <row r="53" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="5" t="n">
         <v>51</v>
       </c>
-      <c r="B53" s="0" t="s">
+      <c r="B53" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="C53" s="0" t="n">
+      <c r="C53" s="6" t="n">
         <v>65</v>
       </c>
-      <c r="D53" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E53" s="0" t="s">
+      <c r="D53" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E53" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="F53" s="0" t="s">
+      <c r="F53" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="G53" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="H53" s="0" t="s">
+      <c r="G53" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H53" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="I53" s="0" t="n">
+      <c r="I53" s="6" t="n">
         <v>0.14</v>
       </c>
-      <c r="J53" s="0" t="n">
+      <c r="J53" s="6" t="n">
         <v>0.14</v>
       </c>
-      <c r="K53" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="L53" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="M53" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N53" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="O53" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="P53" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q53" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="R53" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S53" s="2" t="n">
+      <c r="K53" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="L53" s="6" t="n">
+        <v>50</v>
+      </c>
+      <c r="M53" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N53" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="O53" s="6" t="n">
+        <v>60</v>
+      </c>
+      <c r="P53" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q53" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="R53" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S53" s="6" t="n">
         <v>700</v>
       </c>
-      <c r="T53" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="U53" s="0" t="n">
+      <c r="T53" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="U53" s="6" t="n">
         <v>0.525</v>
       </c>
-      <c r="V53" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="W53" s="0" t="s">
+      <c r="V53" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W53" s="6" t="s">
         <v>150</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix: change cream packing speed
</commit_message>
<xml_diff>
--- a/app/data/static/params/mascarpone.xlsx
+++ b/app/data/static/params/mascarpone.xlsx
@@ -686,8 +686,8 @@
   </sheetPr>
   <dimension ref="A1:W53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V70" activeCellId="0" sqref="V70"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S21" activeCellId="0" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1434,7 +1434,7 @@
         <v>0</v>
       </c>
       <c r="S11" s="4" t="n">
-        <v>1400</v>
+        <v>1680</v>
       </c>
       <c r="T11" s="2" t="n">
         <v>1000</v>
@@ -1502,7 +1502,7 @@
         <v>0</v>
       </c>
       <c r="S12" s="0" t="n">
-        <v>600</v>
+        <v>1250</v>
       </c>
       <c r="T12" s="2" t="n">
         <v>1000</v>
@@ -1570,7 +1570,7 @@
         <v>0</v>
       </c>
       <c r="S13" s="0" t="n">
-        <v>600</v>
+        <v>1250</v>
       </c>
       <c r="T13" s="2" t="n">
         <v>1000</v>
@@ -1845,7 +1845,7 @@
         <v>0</v>
       </c>
       <c r="S17" s="0" t="n">
-        <v>600</v>
+        <v>1680</v>
       </c>
       <c r="T17" s="2" t="n">
         <v>1000</v>
@@ -1981,7 +1981,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="0" t="n">
-        <v>600</v>
+        <v>1250</v>
       </c>
       <c r="T19" s="2" t="n">
         <v>1000</v>

</xml_diff>

<commit_message>
Fix: change mascarpone params and add block_id
</commit_message>
<xml_diff>
--- a/app/data/static/params/mascarpone.xlsx
+++ b/app/data/static/params/mascarpone.xlsx
@@ -513,7 +513,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -524,6 +524,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4C7DC"/>
+        <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -574,7 +580,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -591,10 +597,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -604,6 +606,22 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -632,7 +650,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFB4C7DC"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -686,8 +704,8 @@
   </sheetPr>
   <dimension ref="A1:W53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O54" activeCellId="0" sqref="O54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P19" activeCellId="0" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1381,207 +1399,207 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
+    <row r="11" s="6" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="0" t="n">
+      <c r="B11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="5" t="n">
         <v>38</v>
       </c>
-      <c r="D11" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="0" t="s">
+      <c r="D11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="H11" s="0" t="s">
+      <c r="G11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="I11" s="0" t="n">
+      <c r="I11" s="5" t="n">
         <v>0.5</v>
       </c>
-      <c r="J11" s="0" t="n">
+      <c r="J11" s="5" t="n">
         <v>0.5</v>
       </c>
-      <c r="K11" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="L11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M11" s="0" t="n">
+      <c r="K11" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="L11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="N11" s="5" t="n">
+        <v>45</v>
+      </c>
+      <c r="O11" s="5" t="n">
+        <v>45</v>
+      </c>
+      <c r="P11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" s="7" t="n">
+        <v>1680</v>
+      </c>
+      <c r="T11" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="U11" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="V11" s="5" t="n">
+        <v>-100</v>
+      </c>
+      <c r="W11" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="N11" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="O11" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="P11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="S11" s="4" t="n">
-        <v>1680</v>
-      </c>
-      <c r="T11" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="U11" s="0" t="n">
+      <c r="B12" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" s="5" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="J12" s="5" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="K12" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="L12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="N12" s="5" t="n">
+        <v>45</v>
+      </c>
+      <c r="O12" s="5" t="n">
+        <v>45</v>
+      </c>
+      <c r="P12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" s="5" t="n">
+        <v>1250</v>
+      </c>
+      <c r="T12" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="U12" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="V11" s="0" t="n">
+      <c r="V12" s="5" t="n">
         <v>-100</v>
       </c>
-      <c r="W11" s="0" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="0" t="n">
+      <c r="W12" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="5" t="n">
         <v>38</v>
       </c>
-      <c r="D12" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="0" t="s">
+      <c r="D13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G12" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="I12" s="0" t="n">
+      <c r="G13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I13" s="5" t="n">
         <v>0.25</v>
       </c>
-      <c r="J12" s="0" t="n">
+      <c r="J13" s="5" t="n">
         <v>0.2</v>
       </c>
-      <c r="K12" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="L12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M12" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="N12" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="O12" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="P12" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R12" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="S12" s="0" t="n">
+      <c r="K13" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="L13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="N13" s="5" t="n">
+        <v>45</v>
+      </c>
+      <c r="O13" s="5" t="n">
+        <v>45</v>
+      </c>
+      <c r="P13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" s="5" t="n">
         <v>1250</v>
       </c>
-      <c r="T12" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="U12" s="0" t="n">
+      <c r="T13" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="U13" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="V12" s="0" t="n">
+      <c r="V13" s="5" t="n">
         <v>-100</v>
       </c>
-      <c r="W12" s="0" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="0" t="n">
-        <v>38</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="I13" s="0" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="J13" s="0" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="K13" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="L13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M13" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="N13" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="O13" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="P13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="S13" s="0" t="n">
-        <v>1250</v>
-      </c>
-      <c r="T13" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="U13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="V13" s="0" t="n">
-        <v>-100</v>
-      </c>
-      <c r="W13" s="0" t="s">
+      <c r="W13" s="5" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1792,71 +1810,71 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="n">
+    <row r="17" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="C17" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="D17" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="F17" s="0" t="s">
+      <c r="D17" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G17" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="H17" s="0" t="s">
+      <c r="G17" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="I17" s="0" t="n">
+      <c r="I17" s="5" t="n">
         <v>0.5</v>
       </c>
-      <c r="J17" s="0" t="n">
+      <c r="J17" s="5" t="n">
         <v>0.5</v>
       </c>
-      <c r="K17" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="L17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M17" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="N17" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="O17" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="P17" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R17" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="S17" s="0" t="n">
+      <c r="K17" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="L17" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="N17" s="5" t="n">
+        <v>45</v>
+      </c>
+      <c r="O17" s="5" t="n">
+        <v>45</v>
+      </c>
+      <c r="P17" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R17" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S17" s="5" t="n">
         <v>1680</v>
       </c>
-      <c r="T17" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="U17" s="0" t="n">
+      <c r="T17" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="U17" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="V17" s="0" t="n">
+      <c r="V17" s="5" t="n">
         <v>-100</v>
       </c>
-      <c r="W17" s="0" t="s">
+      <c r="W17" s="5" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1928,71 +1946,71 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
+    <row r="19" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="0" t="n">
+      <c r="C19" s="5" t="n">
         <v>38</v>
       </c>
-      <c r="D19" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="F19" s="0" t="s">
+      <c r="D19" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G19" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="H19" s="0" t="s">
+      <c r="G19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I19" s="0" t="n">
+      <c r="I19" s="5" t="n">
         <v>0.25</v>
       </c>
-      <c r="J19" s="0" t="n">
+      <c r="J19" s="5" t="n">
         <v>0.2</v>
       </c>
-      <c r="K19" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="L19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M19" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="N19" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="O19" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="P19" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R19" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="S19" s="0" t="n">
+      <c r="K19" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="L19" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="N19" s="5" t="n">
+        <v>45</v>
+      </c>
+      <c r="O19" s="5" t="n">
+        <v>45</v>
+      </c>
+      <c r="P19" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R19" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S19" s="5" t="n">
         <v>1250</v>
       </c>
-      <c r="T19" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="U19" s="0" t="n">
+      <c r="T19" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="U19" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="V19" s="0" t="n">
+      <c r="V19" s="5" t="n">
         <v>-100</v>
       </c>
-      <c r="W19" s="0" t="s">
+      <c r="W19" s="5" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2475,139 +2493,139 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="n">
+    <row r="27" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="8" t="n">
         <v>25</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="C27" s="6" t="n">
+      <c r="C27" s="9" t="n">
         <v>65</v>
       </c>
-      <c r="D27" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F27" s="6" t="s">
+      <c r="D27" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="G27" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H27" s="6" t="s">
+      <c r="G27" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H27" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="I27" s="6" t="n">
+      <c r="I27" s="9" t="n">
         <v>0.18</v>
       </c>
-      <c r="J27" s="6" t="n">
+      <c r="J27" s="9" t="n">
         <v>0.2</v>
       </c>
-      <c r="K27" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="L27" s="6" t="n">
-        <v>50</v>
-      </c>
-      <c r="M27" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N27" s="6" t="n">
+      <c r="K27" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="L27" s="9" t="n">
+        <v>50</v>
+      </c>
+      <c r="M27" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N27" s="9" t="n">
         <v>30</v>
       </c>
-      <c r="O27" s="6" t="n">
+      <c r="O27" s="9" t="n">
         <v>60</v>
       </c>
-      <c r="P27" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q27" s="6" t="n">
+      <c r="P27" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="9" t="n">
         <v>30</v>
       </c>
-      <c r="R27" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="S27" s="6" t="n">
+      <c r="R27" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S27" s="9" t="n">
         <v>800</v>
       </c>
-      <c r="T27" s="6" t="n">
-        <v>1000</v>
-      </c>
-      <c r="U27" s="6" t="n">
+      <c r="T27" s="9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="U27" s="9" t="n">
         <v>0.7</v>
       </c>
-      <c r="V27" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="W27" s="6" t="s">
+      <c r="V27" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="W27" s="9" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="28" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5" t="n">
+    <row r="28" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="8" t="n">
         <v>26</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="C28" s="6" t="n">
+      <c r="C28" s="9" t="n">
         <v>65</v>
       </c>
-      <c r="D28" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F28" s="6" t="s">
+      <c r="D28" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="G28" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H28" s="6" t="s">
+      <c r="G28" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H28" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I28" s="6" t="n">
+      <c r="I28" s="9" t="n">
         <v>0.18</v>
       </c>
-      <c r="J28" s="6" t="n">
+      <c r="J28" s="9" t="n">
         <v>0.2</v>
       </c>
-      <c r="K28" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="L28" s="6" t="n">
-        <v>50</v>
-      </c>
-      <c r="M28" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N28" s="6" t="n">
+      <c r="K28" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="L28" s="9" t="n">
+        <v>50</v>
+      </c>
+      <c r="M28" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N28" s="9" t="n">
         <v>30</v>
       </c>
-      <c r="O28" s="6" t="n">
+      <c r="O28" s="9" t="n">
         <v>60</v>
       </c>
-      <c r="P28" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q28" s="6" t="n">
+      <c r="P28" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="9" t="n">
         <v>30</v>
       </c>
-      <c r="R28" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="S28" s="6" t="n">
+      <c r="R28" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S28" s="9" t="n">
         <v>800</v>
       </c>
-      <c r="T28" s="6" t="n">
-        <v>1000</v>
-      </c>
-      <c r="U28" s="6" t="n">
+      <c r="T28" s="9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="U28" s="9" t="n">
         <v>0.7</v>
       </c>
-      <c r="V28" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="W28" s="6" t="s">
+      <c r="V28" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="W28" s="9" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3164,71 +3182,71 @@
         <v>111</v>
       </c>
     </row>
-    <row r="37" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5" t="n">
+    <row r="37" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="8" t="n">
         <v>35</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C37" s="6" t="n">
+      <c r="C37" s="9" t="n">
         <v>65</v>
       </c>
-      <c r="D37" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F37" s="6" t="s">
+      <c r="D37" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F37" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="G37" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H37" s="6" t="s">
+      <c r="G37" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H37" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I37" s="6" t="n">
+      <c r="I37" s="9" t="n">
         <v>0.2</v>
       </c>
-      <c r="J37" s="6" t="n">
+      <c r="J37" s="9" t="n">
         <v>0.2</v>
       </c>
-      <c r="K37" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="L37" s="6" t="n">
-        <v>50</v>
-      </c>
-      <c r="M37" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N37" s="6" t="n">
+      <c r="K37" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="L37" s="9" t="n">
+        <v>50</v>
+      </c>
+      <c r="M37" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N37" s="9" t="n">
         <v>30</v>
       </c>
-      <c r="O37" s="6" t="n">
+      <c r="O37" s="9" t="n">
         <v>60</v>
       </c>
-      <c r="P37" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q37" s="6" t="n">
+      <c r="P37" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="9" t="n">
         <v>30</v>
       </c>
-      <c r="R37" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="S37" s="6" t="n">
+      <c r="R37" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S37" s="9" t="n">
         <v>800</v>
       </c>
-      <c r="T37" s="6" t="n">
-        <v>1000</v>
-      </c>
-      <c r="U37" s="6" t="n">
+      <c r="T37" s="9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="U37" s="9" t="n">
         <v>0.7</v>
       </c>
-      <c r="V37" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="W37" s="6" t="s">
+      <c r="V37" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="W37" s="9" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3646,71 +3664,71 @@
         <v>127</v>
       </c>
     </row>
-    <row r="44" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="5" t="n">
+    <row r="44" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="8" t="n">
         <v>42</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="C44" s="6" t="n">
+      <c r="C44" s="9" t="n">
         <v>65</v>
       </c>
-      <c r="D44" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F44" s="6" t="s">
+      <c r="D44" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F44" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="G44" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H44" s="6" t="s">
+      <c r="G44" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H44" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I44" s="6" t="n">
+      <c r="I44" s="9" t="n">
         <v>0.2</v>
       </c>
-      <c r="J44" s="6" t="n">
+      <c r="J44" s="9" t="n">
         <v>0.2</v>
       </c>
-      <c r="K44" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="L44" s="6" t="n">
-        <v>50</v>
-      </c>
-      <c r="M44" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N44" s="6" t="n">
+      <c r="K44" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="L44" s="9" t="n">
+        <v>50</v>
+      </c>
+      <c r="M44" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N44" s="9" t="n">
         <v>30</v>
       </c>
-      <c r="O44" s="6" t="n">
+      <c r="O44" s="9" t="n">
         <v>60</v>
       </c>
-      <c r="P44" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q44" s="6" t="n">
+      <c r="P44" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="9" t="n">
         <v>30</v>
       </c>
-      <c r="R44" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="S44" s="6" t="n">
+      <c r="R44" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S44" s="9" t="n">
         <v>800</v>
       </c>
-      <c r="T44" s="6" t="n">
-        <v>1000</v>
-      </c>
-      <c r="U44" s="6" t="n">
+      <c r="T44" s="9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="U44" s="9" t="n">
         <v>0.7</v>
       </c>
-      <c r="V44" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="W44" s="6" t="s">
+      <c r="V44" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="W44" s="9" t="s">
         <v>129</v>
       </c>
     </row>
@@ -3921,71 +3939,71 @@
         <v>135</v>
       </c>
     </row>
-    <row r="48" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="5" t="n">
+    <row r="48" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="8" t="n">
         <v>46</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B48" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="C48" s="6" t="n">
+      <c r="C48" s="9" t="n">
         <v>65</v>
       </c>
-      <c r="D48" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F48" s="6" t="s">
+      <c r="D48" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F48" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="G48" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H48" s="6" t="s">
+      <c r="G48" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H48" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I48" s="6" t="n">
+      <c r="I48" s="9" t="n">
         <v>0.25</v>
       </c>
-      <c r="J48" s="6" t="n">
+      <c r="J48" s="9" t="n">
         <v>0.2</v>
       </c>
-      <c r="K48" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="L48" s="6" t="n">
-        <v>50</v>
-      </c>
-      <c r="M48" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N48" s="6" t="n">
+      <c r="K48" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="L48" s="9" t="n">
+        <v>50</v>
+      </c>
+      <c r="M48" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N48" s="9" t="n">
         <v>30</v>
       </c>
-      <c r="O48" s="6" t="n">
+      <c r="O48" s="9" t="n">
         <v>60</v>
       </c>
-      <c r="P48" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q48" s="6" t="n">
+      <c r="P48" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q48" s="9" t="n">
         <v>30</v>
       </c>
-      <c r="R48" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="S48" s="6" t="n">
+      <c r="R48" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S48" s="9" t="n">
         <v>800</v>
       </c>
-      <c r="T48" s="6" t="n">
-        <v>1000</v>
-      </c>
-      <c r="U48" s="6" t="n">
+      <c r="T48" s="9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="U48" s="9" t="n">
         <v>0.7</v>
       </c>
-      <c r="V48" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="W48" s="6" t="s">
+      <c r="V48" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="W48" s="9" t="s">
         <v>137</v>
       </c>
     </row>
@@ -4199,142 +4217,142 @@
         <v>144</v>
       </c>
     </row>
-    <row r="52" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="5" t="n">
-        <v>50</v>
-      </c>
-      <c r="B52" s="6" t="s">
+    <row r="52" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="8" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="C52" s="6" t="n">
+      <c r="C52" s="9" t="n">
         <v>65</v>
       </c>
-      <c r="D52" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F52" s="6" t="s">
+      <c r="D52" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F52" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="G52" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H52" s="6" t="s">
+      <c r="G52" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H52" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="I52" s="6" t="n">
+      <c r="I52" s="9" t="n">
         <v>0.14</v>
       </c>
-      <c r="J52" s="6" t="n">
+      <c r="J52" s="9" t="n">
         <v>0.14</v>
       </c>
-      <c r="K52" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="L52" s="6" t="n">
-        <v>50</v>
-      </c>
-      <c r="M52" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N52" s="6" t="n">
-        <v>20</v>
-      </c>
-      <c r="O52" s="6" t="n">
-        <v>60</v>
-      </c>
-      <c r="P52" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q52" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="R52" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="S52" s="6" t="n">
+      <c r="K52" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="L52" s="9" t="n">
+        <v>50</v>
+      </c>
+      <c r="M52" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N52" s="9" t="n">
+        <v>20</v>
+      </c>
+      <c r="O52" s="9" t="n">
+        <v>50</v>
+      </c>
+      <c r="P52" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q52" s="9" t="n">
+        <v>20</v>
+      </c>
+      <c r="R52" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S52" s="9" t="n">
         <v>700</v>
       </c>
-      <c r="T52" s="6" t="n">
-        <v>1000</v>
-      </c>
-      <c r="U52" s="6" t="n">
+      <c r="T52" s="9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="U52" s="9" t="n">
         <v>0.37</v>
       </c>
-      <c r="V52" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="W52" s="6" t="s">
+      <c r="V52" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="W52" s="9" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="53" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="5" t="n">
+    <row r="53" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="8" t="n">
         <v>51</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="B53" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="C53" s="6" t="n">
+      <c r="C53" s="9" t="n">
         <v>65</v>
       </c>
-      <c r="D53" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E53" s="6" t="s">
+      <c r="D53" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E53" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="F53" s="6" t="s">
+      <c r="F53" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="G53" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H53" s="6" t="s">
+      <c r="G53" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H53" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="I53" s="6" t="n">
+      <c r="I53" s="9" t="n">
         <v>0.14</v>
       </c>
-      <c r="J53" s="6" t="n">
+      <c r="J53" s="9" t="n">
         <v>0.14</v>
       </c>
-      <c r="K53" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="L53" s="6" t="n">
-        <v>50</v>
-      </c>
-      <c r="M53" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N53" s="6" t="n">
-        <v>20</v>
-      </c>
-      <c r="O53" s="6" t="n">
-        <v>60</v>
-      </c>
-      <c r="P53" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q53" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="R53" s="6" t="n">
+      <c r="K53" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="L53" s="9" t="n">
+        <v>50</v>
+      </c>
+      <c r="M53" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N53" s="9" t="n">
+        <v>20</v>
+      </c>
+      <c r="O53" s="9" t="n">
+        <v>50</v>
+      </c>
+      <c r="P53" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q53" s="9" t="n">
+        <v>20</v>
+      </c>
+      <c r="R53" s="9" t="n">
         <v>25</v>
       </c>
-      <c r="S53" s="6" t="n">
+      <c r="S53" s="9" t="n">
         <v>700</v>
       </c>
-      <c r="T53" s="6" t="n">
-        <v>1000</v>
-      </c>
-      <c r="U53" s="6" t="n">
+      <c r="T53" s="9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="U53" s="9" t="n">
         <v>0.395</v>
       </c>
-      <c r="V53" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="W53" s="6" t="s">
+      <c r="V53" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="W53" s="9" t="s">
         <v>150</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update: add new parameters to db
</commit_message>
<xml_diff>
--- a/app/data/static/params/mascarpone.xlsx
+++ b/app/data/static/params/mascarpone.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="173">
   <si>
     <t xml:space="preserve">Название SKU</t>
   </si>
@@ -515,6 +515,30 @@
   </si>
   <si>
     <t xml:space="preserve">00-00011035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Творожный с травами "Вкусвилл", 65%, 0,14 кг, пл/с</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00-00011195</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Творожный "Вкусвилл", 65%, 0,25 кг, пл/с</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00-00011196</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Творожный "Вкусвилл", 65%, 0,14 кг, пл/с</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00-00011197</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Маскарпоне с шоколадом "Бонджорно", 50%, 0,18 кг, пл/с</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00-00011040</t>
   </si>
 </sst>
 </file>
@@ -759,10 +783,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W60"/>
+  <dimension ref="A1:W64"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B52" activeCellId="0" sqref="B52"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E70" activeCellId="0" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4019,10 +4043,10 @@
         <v>28</v>
       </c>
       <c r="I48" s="9" t="n">
-        <v>0.25</v>
+        <v>2.5</v>
       </c>
       <c r="J48" s="9" t="n">
-        <v>0.2</v>
+        <v>2.5</v>
       </c>
       <c r="K48" s="9" t="n">
         <v>6</v>
@@ -4214,7 +4238,7 @@
         <v>143</v>
       </c>
       <c r="C51" s="0" t="n">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="D51" s="0" t="s">
         <v>23</v>
@@ -4901,6 +4925,286 @@
       </c>
       <c r="W60" s="11" t="s">
         <v>164</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="8" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="C61" s="9" t="n">
+        <v>65</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F61" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="G61" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H61" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I61" s="9" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="J61" s="9" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="K61" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="L61" s="9" t="n">
+        <v>50</v>
+      </c>
+      <c r="M61" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N61" s="9" t="n">
+        <v>30</v>
+      </c>
+      <c r="O61" s="9" t="n">
+        <v>60</v>
+      </c>
+      <c r="P61" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q61" s="9" t="n">
+        <v>30</v>
+      </c>
+      <c r="R61" s="9" t="n">
+        <v>25</v>
+      </c>
+      <c r="S61" s="9" t="n">
+        <v>800</v>
+      </c>
+      <c r="T61" s="9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="U61" s="9" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="V61" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="W61" s="12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="8" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="C62" s="9" t="n">
+        <v>65</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E62" s="10"/>
+      <c r="F62" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="G62" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H62" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I62" s="9" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="J62" s="9" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="K62" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="L62" s="9" t="n">
+        <v>50</v>
+      </c>
+      <c r="M62" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N62" s="9" t="n">
+        <v>30</v>
+      </c>
+      <c r="O62" s="9" t="n">
+        <v>60</v>
+      </c>
+      <c r="P62" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q62" s="9" t="n">
+        <v>30</v>
+      </c>
+      <c r="R62" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S62" s="9" t="n">
+        <v>800</v>
+      </c>
+      <c r="T62" s="9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="U62" s="9" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="V62" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="W62" s="12" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="8" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="C63" s="9" t="n">
+        <v>65</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E63" s="10"/>
+      <c r="F63" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="G63" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H63" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I63" s="9" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="J63" s="9" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="K63" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="L63" s="9" t="n">
+        <v>50</v>
+      </c>
+      <c r="M63" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N63" s="9" t="n">
+        <v>30</v>
+      </c>
+      <c r="O63" s="9" t="n">
+        <v>60</v>
+      </c>
+      <c r="P63" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q63" s="9" t="n">
+        <v>30</v>
+      </c>
+      <c r="R63" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S63" s="9" t="n">
+        <v>800</v>
+      </c>
+      <c r="T63" s="9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="U63" s="9" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="V63" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="W63" s="12" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="8" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="C64" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E64" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F64" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G64" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H64" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="I64" s="0" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="J64" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="K64" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="L64" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="M64" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N64" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="O64" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="P64" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q64" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R64" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="S64" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="T64" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="U64" s="0" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="V64" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W64" s="11" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update mascarpone batch number logic
</commit_message>
<xml_diff>
--- a/app/data/static/params/mascarpone.xlsx
+++ b/app/data/static/params/mascarpone.xlsx
@@ -634,7 +634,7 @@
   <dimension ref="A1:W43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q42" activeCellId="0" sqref="Q42"/>
+      <selection pane="topLeft" activeCell="S36" activeCellId="0" sqref="S36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3109,10 +3109,10 @@
         <v>300</v>
       </c>
       <c r="T36" s="3" t="n">
-        <v>1200</v>
+        <v>1000</v>
       </c>
       <c r="U36" s="3" t="n">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="V36" s="3" t="n">
         <v>0</v>

</xml_diff>